<commit_message>
Modif script user + poid scrum
J'ai aussi taper les ressources dans un dossier séparer pour pas trop
s'y perdre
</commit_message>
<xml_diff>
--- a/Scrum final.xlsx
+++ b/Scrum final.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\Dossier-SGBD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>STORIES</t>
   </si>
@@ -28,9 +33,6 @@
     <t>FAIT</t>
   </si>
   <si>
-    <t>Création des bases de données CB et CBB light - XL</t>
-  </si>
-  <si>
     <t>Créer le schéma relationnel (infos des users, leurs cotes et avis sur les films + date =&gt; pas de FK vers films à ce moment) /!\ stocker infos data warehouse</t>
   </si>
   <si>
@@ -64,18 +66,12 @@
     <t>Recopie des modifs faites dans CBB pour assurer l'équivalence</t>
   </si>
   <si>
-    <t>Création de CB et CBB - XL</t>
-  </si>
-  <si>
     <t>Etendre le script de création en y intégrant les films et données associées</t>
   </si>
   <si>
     <t>Rapport des statistiques (package UTL_FILE)</t>
   </si>
   <si>
-    <t>Alimentation de CB - XL</t>
-  </si>
-  <si>
     <t>Calcul 99ème percentile</t>
   </si>
   <si>
@@ -136,9 +132,6 @@
     <t>Ajouter à la recherche le critère des n meilleurs films selon le nombre de cotes des users (n entré)</t>
   </si>
   <si>
-    <t>Simulation d'un plantage de CB - L</t>
-  </si>
-  <si>
     <t>Localiser la session de l'utilisateur</t>
   </si>
   <si>
@@ -154,15 +147,9 @@
     <t>Si au milieu d'une opération =&gt; ROLLBACK, prévenir le user qui recommence</t>
   </si>
   <si>
-    <t>Sauvegarde des informations de CB - M</t>
-  </si>
-  <si>
     <t>Etendre BackupCBLight aux films et infos liées (asynchrone) et aux copies (synchrone)</t>
   </si>
   <si>
-    <t>Restauration des informations de CB - M</t>
-  </si>
-  <si>
     <t>Dans les procédures stockées de CBB, vérifier si CB est redevenu utilisable =&gt; msg à l'app</t>
   </si>
   <si>
@@ -199,9 +186,6 @@
     <t>Envoyer les cotes et avis du film mais pas l'utilisateur qui a rédigé</t>
   </si>
   <si>
-    <t>Retour des copies - S</t>
-  </si>
-  <si>
     <t>Même si le film n'a plus de copie, on garde sa signalétique dans CC pour les archives</t>
   </si>
   <si>
@@ -229,9 +213,6 @@
     <t>Conserver trace de tous les films (nombre de jours à l'affiche, nombres de places vendues, nombre de copies manipulées)</t>
   </si>
   <si>
-    <t>Recherche de places libres - L</t>
-  </si>
-  <si>
     <t>Recherche (parmi la programmation) sur popularité, pérennité, position dans palmarès, titre, genre</t>
   </si>
   <si>
@@ -244,9 +225,6 @@
     <t>Affichage conçu pour permettre la commande de places</t>
   </si>
   <si>
-    <t>Commande de places - M</t>
-  </si>
-  <si>
     <t>A partir de la recherche de places, fonctionnalité de "panier" (nbr de places à insérer)</t>
   </si>
   <si>
@@ -265,9 +243,6 @@
     <t>Attention au suivi de l'information : affichages etc pour tenir le user au courant</t>
   </si>
   <si>
-    <t>Génération de tickets - M</t>
-  </si>
-  <si>
     <t>Quand commande validée =&gt; génération d'un doc pdf (stocké sur MongoDB) contenant les infos des films et QR codes</t>
   </si>
   <si>
@@ -283,9 +258,6 @@
     <t>Suivi de log</t>
   </si>
   <si>
-    <t>Détail des signalétiques d'acteurs - S</t>
-  </si>
-  <si>
     <t>Créer la BD BP</t>
   </si>
   <si>
@@ -334,9 +306,6 @@
     <t>Slicing, scoping, roll up, drill down</t>
   </si>
   <si>
-    <t>Dossier installation, mise en route, exploitation - L</t>
-  </si>
-  <si>
     <t>Garder les MCD et MRD au propre</t>
   </si>
   <si>
@@ -358,18 +327,12 @@
     <t>Script d'installation ?</t>
   </si>
   <si>
-    <t>Maintenance, mise à jour - L</t>
-  </si>
-  <si>
     <t>Faire une présentation générale des différents fichiers et packages + leur organisation (flèches, couleurs etc)</t>
   </si>
   <si>
     <t>COMMENTAIRES (IN/OUT/PROCESS + blocs plus complexes)</t>
   </si>
   <si>
-    <t>Sauvegarde et récupération - L</t>
-  </si>
-  <si>
     <t>Faire un plan général de ce qu'est un plan de sauvegarde et/ou récupération</t>
   </si>
   <si>
@@ -380,13 +343,58 @@
   </si>
   <si>
     <t>Archivage des programmations - S</t>
+  </si>
+  <si>
+    <t>Création des bases de données CB et CBB light - S</t>
+  </si>
+  <si>
+    <t>Alimentation de CB - L</t>
+  </si>
+  <si>
+    <t>Création de CB et CBB - S</t>
+  </si>
+  <si>
+    <t>Vu que la table film sera créée en fonction de l'analyse du fichier film (calcul percentilen, etc ) il vaudrait mieux faire cette storie après celle d'en dessous</t>
+  </si>
+  <si>
+    <t>Simulation d'un plantage de CB - M</t>
+  </si>
+  <si>
+    <t>Sauvegarde des informations de CB - L</t>
+  </si>
+  <si>
+    <t>Restauration des informations de CB - L</t>
+  </si>
+  <si>
+    <t>Retour des copies - M</t>
+  </si>
+  <si>
+    <t>Recherche de places libres - M</t>
+  </si>
+  <si>
+    <t>Commande de places - XL</t>
+  </si>
+  <si>
+    <t>Génération de tickets - XL</t>
+  </si>
+  <si>
+    <t>Sauvegarde et récupération - S</t>
+  </si>
+  <si>
+    <t>Maintenance, mise à jour - S</t>
+  </si>
+  <si>
+    <t>Dossier installation, mise en route, exploitation - S</t>
+  </si>
+  <si>
+    <t>Détail des signalétiques d'acteurs - M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +414,13 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -577,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -639,22 +654,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -663,11 +681,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -709,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,9 +767,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,6 +802,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -950,21 +978,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" style="23" customWidth="1"/>
     <col min="2" max="4" width="70.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -978,973 +1006,962 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="7"/>
       <c r="C2" s="5"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="22"/>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A5" s="23"/>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
       <c r="B5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A6" s="24"/>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="21" t="s">
-        <v>10</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A9" s="24"/>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
       <c r="B9" s="9"/>
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>12</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
       <c r="B11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="22"/>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
       <c r="B12" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
       <c r="B13" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A14" s="24"/>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="21" t="s">
-        <v>16</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A16" s="23"/>
+    <row r="16" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>111</v>
+      </c>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A17" s="24"/>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="21" t="s">
-        <v>19</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="22"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A20" s="23"/>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="21" t="s">
-        <v>23</v>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="22"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
       <c r="B23" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A24" s="23"/>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="21" t="s">
-        <v>27</v>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="22"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
       <c r="B27" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
       <c r="B28" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A29" s="23"/>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25"/>
       <c r="B29" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A30" s="24"/>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
       <c r="B30" s="9"/>
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="21" t="s">
-        <v>32</v>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>29</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="22"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
       <c r="B32" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="22"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
       <c r="B33" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A34" s="23"/>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
       <c r="B34" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A35" s="24"/>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
       <c r="B35" s="9"/>
       <c r="C35" s="6"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" ht="30">
-      <c r="A36" s="21" t="s">
-        <v>37</v>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
     </row>
-    <row r="37" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A37" s="23"/>
+    <row r="37" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
       <c r="B37" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A38" s="24"/>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
       <c r="B38" s="9"/>
       <c r="C38" s="6"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1">
-      <c r="A39" s="21" t="s">
-        <v>40</v>
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="22"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="22"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="22"/>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
       <c r="B42" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A43" s="23"/>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25"/>
       <c r="B43" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="12"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A44" s="24"/>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
       <c r="B44" s="9"/>
       <c r="C44" s="6"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A45" s="25" t="s">
-        <v>46</v>
+    <row r="45" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="19"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A46" s="24"/>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="21" t="s">
-        <v>48</v>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="16"/>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="22"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
       <c r="B48" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A49" s="23"/>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25"/>
       <c r="B49" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="12"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A50" s="24"/>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="21"/>
       <c r="B50" s="9"/>
       <c r="C50" s="6"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="21" t="s">
-        <v>52</v>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A52" s="23"/>
+    <row r="52" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25"/>
       <c r="B52" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="12"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A53" s="24"/>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
       <c r="B53" s="9"/>
       <c r="C53" s="6"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="21" t="s">
-        <v>55</v>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="16"/>
     </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="22"/>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
       <c r="B55" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="22"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
       <c r="B56" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="22"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="26"/>
       <c r="B57" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A58" s="23"/>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="25"/>
       <c r="B58" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="12"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A59" s="24"/>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
       <c r="B59" s="9"/>
       <c r="C59" s="6"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="21" t="s">
-        <v>61</v>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="16"/>
     </row>
-    <row r="61" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A61" s="23"/>
+    <row r="61" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="25"/>
       <c r="B61" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="12"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A62" s="24"/>
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="21"/>
       <c r="B62" s="9"/>
       <c r="C62" s="6"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="21" t="s">
-        <v>64</v>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
     </row>
-    <row r="64" spans="1:4" ht="30">
-      <c r="A64" s="22"/>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="26"/>
       <c r="B64" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="1:4" ht="30">
-      <c r="A65" s="22"/>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="26"/>
       <c r="B65" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="22"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="26"/>
       <c r="B66" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="22"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="26"/>
       <c r="B67" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A68" s="23"/>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="25"/>
       <c r="B68" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A69" s="24"/>
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="21"/>
       <c r="B69" s="9"/>
       <c r="C69" s="6"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A70" s="25" t="s">
-        <v>121</v>
+    <row r="70" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A71" s="24"/>
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="21"/>
       <c r="B71" s="9"/>
       <c r="C71" s="6"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="1:4" ht="30">
-      <c r="A72" s="21" t="s">
-        <v>71</v>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
+        <v>116</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="16"/>
     </row>
-    <row r="73" spans="1:4" ht="30">
-      <c r="A73" s="22"/>
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="26"/>
       <c r="B73" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="22"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="26"/>
       <c r="B74" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A75" s="23"/>
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="25"/>
       <c r="B75" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="12"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A76" s="24"/>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="21"/>
       <c r="B76" s="9"/>
       <c r="C76" s="6"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="1:4" ht="30">
-      <c r="A77" s="21" t="s">
-        <v>76</v>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="16"/>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="22"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="26"/>
       <c r="B78" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="1:4" ht="30">
-      <c r="A79" s="22"/>
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="26"/>
       <c r="B79" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:4" ht="30">
-      <c r="A80" s="22"/>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="26"/>
       <c r="B80" s="9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="22"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="26"/>
       <c r="B81" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A82" s="23"/>
+    <row r="82" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="25"/>
       <c r="B82" s="11" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="12"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A83" s="24"/>
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21"/>
       <c r="B83" s="9"/>
       <c r="C83" s="6"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="1:4" ht="30">
-      <c r="A84" s="21" t="s">
-        <v>83</v>
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="16"/>
     </row>
-    <row r="85" spans="1:4" ht="30">
-      <c r="A85" s="22"/>
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="26"/>
       <c r="B85" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="22"/>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="26"/>
       <c r="B86" s="9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="22"/>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="26"/>
       <c r="B87" s="9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A88" s="23"/>
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="25"/>
       <c r="B88" s="11" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="12"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A89" s="24"/>
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="21"/>
       <c r="B89" s="9"/>
       <c r="C89" s="6"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="1:4" ht="30" customHeight="1">
-      <c r="A90" s="21" t="s">
-        <v>89</v>
+    <row r="90" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="16"/>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="22"/>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="26"/>
       <c r="B91" s="9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A92" s="23"/>
+    <row r="92" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="25"/>
       <c r="B92" s="11" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="12"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A93" s="24"/>
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="21"/>
       <c r="B93" s="9"/>
       <c r="C93" s="6"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="1:4" ht="30" customHeight="1">
-      <c r="A94" s="21" t="s">
-        <v>93</v>
+    <row r="94" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="24" t="s">
+        <v>82</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C94" s="15"/>
       <c r="D94" s="16"/>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="22"/>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="26"/>
       <c r="B95" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="1:4" ht="30">
-      <c r="A96" s="22"/>
+    <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="26"/>
       <c r="B96" s="9" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A97" s="23"/>
+    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="25"/>
       <c r="B97" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="12"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A98" s="24"/>
+    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="21"/>
       <c r="B98" s="9"/>
       <c r="C98" s="6"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A99" s="25" t="s">
-        <v>98</v>
+    <row r="99" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="19"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A100" s="24"/>
+    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="21"/>
       <c r="B100" s="9"/>
       <c r="C100" s="6"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A101" s="25" t="s">
-        <v>100</v>
+    <row r="101" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C101" s="18"/>
       <c r="D101" s="19"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A102" s="24"/>
+    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="21"/>
       <c r="B102" s="9"/>
       <c r="C102" s="6"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="1:4" ht="30" customHeight="1">
-      <c r="A103" s="21" t="s">
-        <v>102</v>
+    <row r="103" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="24" t="s">
+        <v>91</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="22"/>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="26"/>
       <c r="B104" s="9" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C104" s="6"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A105" s="23"/>
+    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="25"/>
       <c r="B105" s="11" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="12"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A106" s="24"/>
+    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="21"/>
       <c r="B106" s="9"/>
       <c r="C106" s="6"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="1:4" ht="30" customHeight="1">
-      <c r="A107" s="21" t="s">
-        <v>106</v>
+    <row r="107" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="24" t="s">
+        <v>121</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="16"/>
     </row>
-    <row r="108" spans="1:4" ht="30">
-      <c r="A108" s="22"/>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="26"/>
       <c r="B108" s="9" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="1:4" ht="30">
-      <c r="A109" s="22"/>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="26"/>
       <c r="B109" s="9" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="1:4" ht="30">
-      <c r="A110" s="22"/>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="26"/>
       <c r="B110" s="9" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="22"/>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="26"/>
       <c r="B111" s="9" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C111" s="6"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="22"/>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="26"/>
       <c r="B112" s="9" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C112" s="6"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A113" s="23"/>
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="25"/>
       <c r="B113" s="11" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C113" s="13"/>
       <c r="D113" s="12"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A114" s="24"/>
+    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="21"/>
       <c r="B114" s="9"/>
       <c r="C114" s="6"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="1:4" ht="30">
-      <c r="A115" s="21" t="s">
-        <v>114</v>
+    <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="16"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A116" s="23"/>
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="25"/>
       <c r="B116" s="11" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C116" s="13"/>
       <c r="D116" s="12"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A117" s="24"/>
+    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="21"/>
       <c r="B117" s="9"/>
       <c r="C117" s="6"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="21" t="s">
-        <v>117</v>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C118" s="15"/>
       <c r="D118" s="16"/>
     </row>
-    <row r="119" spans="1:4" ht="30">
-      <c r="A119" s="22"/>
+    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="26"/>
       <c r="B119" s="9" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A120" s="23"/>
+    <row r="120" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="25"/>
       <c r="B120" s="11" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C120" s="13"/>
       <c r="D120" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A77:A82"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A107:A113"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A63:A68"/>
     <mergeCell ref="A72:A75"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A36:A37"/>
@@ -1956,6 +1973,19 @@
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A107:A113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise au propre scrum (échange des stories)
</commit_message>
<xml_diff>
--- a/Scrum final.xlsx
+++ b/Scrum final.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\Dossier-SGBD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>STORIES</t>
   </si>
@@ -66,9 +61,6 @@
     <t>Recopie des modifs faites dans CBB pour assurer l'équivalence</t>
   </si>
   <si>
-    <t>Etendre le script de création en y intégrant les films et données associées</t>
-  </si>
-  <si>
     <t>Rapport des statistiques (package UTL_FILE)</t>
   </si>
   <si>
@@ -354,9 +346,6 @@
     <t>Création de CB et CBB - S</t>
   </si>
   <si>
-    <t>Vu que la table film sera créée en fonction de l'analyse du fichier film (calcul percentilen, etc ) il vaudrait mieux faire cette storie après celle d'en dessous</t>
-  </si>
-  <si>
     <t>Simulation d'un plantage de CB - M</t>
   </si>
   <si>
@@ -388,13 +377,16 @@
   </si>
   <si>
     <t>Détail des signalétiques d'acteurs - M</t>
+  </si>
+  <si>
+    <t>Etendre le script de création en y intégrant les films et données associées (calcul math)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +655,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,9 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,7 +685,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -735,7 +727,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,10 +759,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -802,7 +793,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -978,21 +968,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:A92"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.7109375" style="23" customWidth="1"/>
     <col min="2" max="4" width="70.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="24" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1006,15 +996,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="20"/>
       <c r="B2" s="7"/>
       <c r="C2" s="5"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>108</v>
+    <row r="3" spans="1:4" ht="30">
+      <c r="A3" s="25" t="s">
+        <v>107</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>4</v>
@@ -1022,30 +1012,30 @@
       <c r="C3" s="15"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="27"/>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A5" s="26"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="21"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -1054,22 +1044,22 @@
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A8" s="26"/>
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
       <c r="A9" s="21"/>
       <c r="B9" s="9"/>
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -1078,884 +1068,882 @@
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:4">
+      <c r="A11" s="27"/>
       <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="27"/>
       <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A13" s="26"/>
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1">
       <c r="A14" s="21"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>110</v>
+    <row r="15" spans="1:4">
+      <c r="A15" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="27"/>
+      <c r="B16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A17" s="26"/>
+      <c r="B17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" ht="30">
+      <c r="A19" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+      <c r="B19" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A20" s="26"/>
       <c r="B20" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
       <c r="A21" s="21"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:4" ht="30">
+      <c r="A22" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>21</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:4">
+      <c r="A23" s="27"/>
       <c r="B23" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A24" s="26"/>
       <c r="B24" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1">
       <c r="A25" s="21"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>25</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:4">
+      <c r="A27" s="27"/>
       <c r="B27" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:4">
+      <c r="A28" s="27"/>
       <c r="B28" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A29" s="26"/>
       <c r="B29" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1">
       <c r="A30" s="21"/>
       <c r="B30" s="9"/>
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:4" ht="30">
+      <c r="A31" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+    <row r="32" spans="1:4">
+      <c r="A32" s="27"/>
       <c r="B32" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+    <row r="33" spans="1:4">
+      <c r="A33" s="27"/>
       <c r="B33" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A34" s="26"/>
       <c r="B34" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1">
       <c r="A35" s="21"/>
       <c r="B35" s="9"/>
       <c r="C35" s="6"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:4" ht="30">
+      <c r="A36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
     </row>
-    <row r="37" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
+    <row r="37" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A37" s="26"/>
       <c r="B37" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1">
       <c r="A38" s="21"/>
       <c r="B38" s="9"/>
       <c r="C38" s="6"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>112</v>
+    <row r="39" spans="1:4" ht="30" customHeight="1">
+      <c r="A39" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:4">
+      <c r="A40" s="27"/>
       <c r="B40" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+    <row r="41" spans="1:4">
+      <c r="A41" s="27"/>
       <c r="B41" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+    <row r="42" spans="1:4" ht="30">
+      <c r="A42" s="27"/>
       <c r="B42" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A43" s="26"/>
       <c r="B43" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="12"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
       <c r="A44" s="21"/>
       <c r="B44" s="9"/>
       <c r="C44" s="6"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="30.75" thickBot="1">
       <c r="A45" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="19"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
       <c r="A46" s="21"/>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>114</v>
+    <row r="47" spans="1:4" ht="30">
+      <c r="A47" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="16"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+    <row r="48" spans="1:4">
+      <c r="A48" s="27"/>
       <c r="B48" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="25"/>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A49" s="26"/>
       <c r="B49" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="12"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1">
       <c r="A50" s="21"/>
       <c r="B50" s="9"/>
       <c r="C50" s="6"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+    <row r="51" spans="1:4">
+      <c r="A51" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="25"/>
+    <row r="52" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A52" s="26"/>
       <c r="B52" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="12"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
       <c r="A53" s="21"/>
       <c r="B53" s="9"/>
       <c r="C53" s="6"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+    <row r="54" spans="1:4" ht="30">
+      <c r="A54" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="16"/>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+    <row r="55" spans="1:4" ht="30">
+      <c r="A55" s="27"/>
       <c r="B55" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+    <row r="56" spans="1:4">
+      <c r="A56" s="27"/>
       <c r="B56" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+    <row r="57" spans="1:4">
+      <c r="A57" s="27"/>
       <c r="B57" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="25"/>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A58" s="26"/>
       <c r="B58" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="12"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1">
       <c r="A59" s="21"/>
       <c r="B59" s="9"/>
       <c r="C59" s="6"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
-        <v>115</v>
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="16"/>
     </row>
-    <row r="61" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="25"/>
+    <row r="61" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A61" s="26"/>
       <c r="B61" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="12"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1">
       <c r="A62" s="21"/>
       <c r="B62" s="9"/>
       <c r="C62" s="6"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+    <row r="63" spans="1:4">
+      <c r="A63" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
     </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+    <row r="64" spans="1:4" ht="30">
+      <c r="A64" s="27"/>
       <c r="B64" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
+    <row r="65" spans="1:4" ht="30">
+      <c r="A65" s="27"/>
       <c r="B65" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+    <row r="66" spans="1:4">
+      <c r="A66" s="27"/>
       <c r="B66" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
+    <row r="67" spans="1:4">
+      <c r="A67" s="27"/>
       <c r="B67" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="25"/>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A68" s="26"/>
       <c r="B68" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1">
       <c r="A69" s="21"/>
       <c r="B69" s="9"/>
       <c r="C69" s="6"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="30.75" thickBot="1">
       <c r="A70" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" thickBot="1">
       <c r="A71" s="21"/>
       <c r="B71" s="9"/>
       <c r="C71" s="6"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
-        <v>116</v>
+    <row r="72" spans="1:4" ht="30">
+      <c r="A72" s="25" t="s">
+        <v>114</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="16"/>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
+    <row r="73" spans="1:4" ht="30">
+      <c r="A73" s="27"/>
       <c r="B73" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+    <row r="74" spans="1:4">
+      <c r="A74" s="27"/>
       <c r="B74" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="25"/>
+    <row r="75" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A75" s="26"/>
       <c r="B75" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="12"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.75" thickBot="1">
       <c r="A76" s="21"/>
       <c r="B76" s="9"/>
       <c r="C76" s="6"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
-        <v>117</v>
+    <row r="77" spans="1:4" ht="30">
+      <c r="A77" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="16"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
+    <row r="78" spans="1:4">
+      <c r="A78" s="27"/>
       <c r="B78" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
+    <row r="79" spans="1:4" ht="30">
+      <c r="A79" s="27"/>
       <c r="B79" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+    <row r="80" spans="1:4" ht="30">
+      <c r="A80" s="27"/>
       <c r="B80" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
+    <row r="81" spans="1:4">
+      <c r="A81" s="27"/>
       <c r="B81" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="25"/>
+    <row r="82" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A82" s="26"/>
       <c r="B82" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="12"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="15.75" thickBot="1">
       <c r="A83" s="21"/>
       <c r="B83" s="9"/>
       <c r="C83" s="6"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
-        <v>118</v>
+    <row r="84" spans="1:4" ht="30">
+      <c r="A84" s="25" t="s">
+        <v>116</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="16"/>
     </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+    <row r="85" spans="1:4" ht="30">
+      <c r="A85" s="27"/>
       <c r="B85" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
+    <row r="86" spans="1:4">
+      <c r="A86" s="27"/>
       <c r="B86" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+    <row r="87" spans="1:4">
+      <c r="A87" s="27"/>
       <c r="B87" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="25"/>
+    <row r="88" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A88" s="26"/>
       <c r="B88" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="12"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15.75" thickBot="1">
       <c r="A89" s="21"/>
       <c r="B89" s="9"/>
       <c r="C89" s="6"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="24" t="s">
-        <v>122</v>
+    <row r="90" spans="1:4" ht="30" customHeight="1">
+      <c r="A90" s="25" t="s">
+        <v>120</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="16"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+    <row r="91" spans="1:4">
+      <c r="A91" s="27"/>
       <c r="B91" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="25"/>
+    <row r="92" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A92" s="26"/>
       <c r="B92" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="12"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="15.75" thickBot="1">
       <c r="A93" s="21"/>
       <c r="B93" s="9"/>
       <c r="C93" s="6"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="24" t="s">
+    <row r="94" spans="1:4" ht="30" customHeight="1">
+      <c r="A94" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="C94" s="15"/>
       <c r="D94" s="16"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+    <row r="95" spans="1:4">
+      <c r="A95" s="27"/>
       <c r="B95" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
+    <row r="96" spans="1:4" ht="30">
+      <c r="A96" s="27"/>
       <c r="B96" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="25"/>
+    <row r="97" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A97" s="26"/>
       <c r="B97" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="12"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" thickBot="1">
       <c r="A98" s="21"/>
       <c r="B98" s="9"/>
       <c r="C98" s="6"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="30.75" thickBot="1">
       <c r="A99" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="B99" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="19"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="15.75" thickBot="1">
       <c r="A100" s="21"/>
       <c r="B100" s="9"/>
       <c r="C100" s="6"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="30.75" thickBot="1">
       <c r="A101" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B101" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="C101" s="18"/>
       <c r="D101" s="19"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="15.75" thickBot="1">
       <c r="A102" s="21"/>
       <c r="B102" s="9"/>
       <c r="C102" s="6"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="24" t="s">
+    <row r="103" spans="1:4" ht="30" customHeight="1">
+      <c r="A103" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>92</v>
       </c>
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
+    <row r="104" spans="1:4">
+      <c r="A104" s="27"/>
       <c r="B104" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C104" s="6"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="25"/>
+    <row r="105" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A105" s="26"/>
       <c r="B105" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="12"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.75" thickBot="1">
       <c r="A106" s="21"/>
       <c r="B106" s="9"/>
       <c r="C106" s="6"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="24" t="s">
-        <v>121</v>
+    <row r="107" spans="1:4" ht="30" customHeight="1">
+      <c r="A107" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="16"/>
     </row>
-    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
+    <row r="108" spans="1:4" ht="30">
+      <c r="A108" s="27"/>
       <c r="B108" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
+    <row r="109" spans="1:4" ht="30">
+      <c r="A109" s="27"/>
       <c r="B109" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
+    <row r="110" spans="1:4" ht="30">
+      <c r="A110" s="27"/>
       <c r="B110" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
+    <row r="111" spans="1:4">
+      <c r="A111" s="27"/>
       <c r="B111" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C111" s="6"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
+    <row r="112" spans="1:4">
+      <c r="A112" s="27"/>
       <c r="B112" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C112" s="6"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="25"/>
+    <row r="113" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A113" s="26"/>
       <c r="B113" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C113" s="13"/>
       <c r="D113" s="12"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="15.75" thickBot="1">
       <c r="A114" s="21"/>
       <c r="B114" s="9"/>
       <c r="C114" s="6"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="24" t="s">
-        <v>120</v>
+    <row r="115" spans="1:4" ht="30">
+      <c r="A115" s="25" t="s">
+        <v>118</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="16"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="25"/>
+    <row r="116" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A116" s="26"/>
       <c r="B116" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C116" s="13"/>
       <c r="D116" s="12"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1">
       <c r="A117" s="21"/>
       <c r="B117" s="9"/>
       <c r="C117" s="6"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="24" t="s">
-        <v>119</v>
+    <row r="118" spans="1:4">
+      <c r="A118" s="25" t="s">
+        <v>117</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C118" s="15"/>
       <c r="D118" s="16"/>
     </row>
-    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
+    <row r="119" spans="1:4" ht="30">
+      <c r="A119" s="27"/>
       <c r="B119" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="25"/>
+    <row r="120" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A120" s="26"/>
       <c r="B120" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C120" s="13"/>
       <c r="D120" s="12"/>
@@ -1969,8 +1957,8 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A47:A49"/>

</xml_diff>

<commit_message>
Le format DATE n'affiche que le jour par défaut. Pour voir si les heures ont été ajoutées : SELECT TO_CHAR(DATEEVAL, 'DD/MM/YYYY HH24:MI:SS') FROM EVALUATION;
</commit_message>
<xml_diff>
--- a/Scrum final.xlsx
+++ b/Scrum final.xlsx
@@ -379,7 +379,7 @@
     <t>Détail des signalétiques d'acteurs - M</t>
   </si>
   <si>
-    <t>Etendre le script de création en y intégrant les films et données associées (calcul math)</t>
+    <t>Etendre le script de création en y intégrant les films et données associées (calcul math) /!\ stocker infos data warehouse</t>
   </si>
 </sst>
 </file>
@@ -661,10 +661,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1006,27 +1006,27 @@
       <c r="A3" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="27"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="21"/>
@@ -1038,14 +1038,14 @@
       <c r="A7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15"/>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="27"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="27"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="11" t="s">
         <v>15</v>
       </c>
@@ -1165,7 +1165,7 @@
       <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="11" t="s">
         <v>22</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="D26" s="16"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="9" t="s">
         <v>25</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="9" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1213,7 @@
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A29" s="26"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="11" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="27"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="27"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A34" s="26"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="11" t="s">
         <v>32</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A37" s="26"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="D39" s="16"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="27"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
         <v>37</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="27"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="27"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="9" t="s">
         <v>39</v>
       </c>
@@ -1325,7 +1325,7 @@
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="11" t="s">
         <v>40</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="D47" s="16"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="27"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="9" t="s">
         <v>43</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A49" s="26"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="11" t="s">
         <v>44</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="D51" s="16"/>
     </row>
     <row r="52" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A52" s="26"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="11" t="s">
         <v>47</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="D54" s="16"/>
     </row>
     <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="27"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="9" t="s">
         <v>50</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="27"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="9" t="s">
         <v>51</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="27"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="9" t="s">
         <v>52</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A58" s="26"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="11" t="s">
         <v>53</v>
       </c>
@@ -1469,7 +1469,7 @@
       <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A61" s="26"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="11" t="s">
         <v>55</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" ht="30">
-      <c r="A64" s="27"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="9" t="s">
         <v>58</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" ht="30">
-      <c r="A65" s="27"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="9" t="s">
         <v>59</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="D65" s="10"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="27"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="9" t="s">
         <v>60</v>
       </c>
@@ -1517,7 +1517,7 @@
       <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="27"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="9" t="s">
         <v>51</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A68" s="26"/>
+      <c r="A68" s="27"/>
       <c r="B68" s="11" t="s">
         <v>61</v>
       </c>
@@ -1565,7 +1565,7 @@
       <c r="D72" s="16"/>
     </row>
     <row r="73" spans="1:4" ht="30">
-      <c r="A73" s="27"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="9" t="s">
         <v>64</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="27"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="9" t="s">
         <v>65</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A75" s="26"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="11" t="s">
         <v>66</v>
       </c>
@@ -1605,7 +1605,7 @@
       <c r="D77" s="16"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="27"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="9" t="s">
         <v>68</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" ht="30">
-      <c r="A79" s="27"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="9" t="s">
         <v>69</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4" ht="30">
-      <c r="A80" s="27"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="9" t="s">
         <v>70</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="27"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="9" t="s">
         <v>71</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A82" s="26"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="11" t="s">
         <v>72</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="D84" s="16"/>
     </row>
     <row r="85" spans="1:4" ht="30">
-      <c r="A85" s="27"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="9" t="s">
         <v>74</v>
       </c>
@@ -1669,7 +1669,7 @@
       <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="27"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="9" t="s">
         <v>75</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="D86" s="10"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="27"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="9" t="s">
         <v>76</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="D87" s="10"/>
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A88" s="26"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="11" t="s">
         <v>77</v>
       </c>
@@ -1709,7 +1709,7 @@
       <c r="D90" s="16"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="27"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="9" t="s">
         <v>80</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A92" s="26"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="11" t="s">
         <v>79</v>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="D94" s="16"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="27"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="9" t="s">
         <v>83</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="D95" s="10"/>
     </row>
     <row r="96" spans="1:4" ht="30">
-      <c r="A96" s="27"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="9" t="s">
         <v>84</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A97" s="26"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="11" t="s">
         <v>85</v>
       </c>
@@ -1813,7 +1813,7 @@
       <c r="D103" s="16"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="27"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="9" t="s">
         <v>92</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="D104" s="10"/>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A105" s="26"/>
+      <c r="A105" s="27"/>
       <c r="B105" s="11" t="s">
         <v>93</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="D107" s="16"/>
     </row>
     <row r="108" spans="1:4" ht="30">
-      <c r="A108" s="27"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="9" t="s">
         <v>95</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="D108" s="10"/>
     </row>
     <row r="109" spans="1:4" ht="30">
-      <c r="A109" s="27"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="9" t="s">
         <v>96</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:4" ht="30">
-      <c r="A110" s="27"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="9" t="s">
         <v>97</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="D110" s="10"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="27"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="9" t="s">
         <v>98</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="D111" s="10"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="27"/>
+      <c r="A112" s="26"/>
       <c r="B112" s="9" t="s">
         <v>99</v>
       </c>
@@ -1885,7 +1885,7 @@
       <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A113" s="26"/>
+      <c r="A113" s="27"/>
       <c r="B113" s="11" t="s">
         <v>100</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="D115" s="16"/>
     </row>
     <row r="116" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A116" s="26"/>
+      <c r="A116" s="27"/>
       <c r="B116" s="11" t="s">
         <v>102</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="D118" s="16"/>
     </row>
     <row r="119" spans="1:4" ht="30">
-      <c r="A119" s="27"/>
+      <c r="A119" s="26"/>
       <c r="B119" s="9" t="s">
         <v>104</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="D119" s="10"/>
     </row>
     <row r="120" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A120" s="26"/>
+      <c r="A120" s="27"/>
       <c r="B120" s="11" t="s">
         <v>105</v>
       </c>
@@ -1950,6 +1950,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A107:A113"/>
     <mergeCell ref="A72:A75"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A36:A37"/>
@@ -1966,14 +1974,6 @@
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A77:A82"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A107:A113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>